<commit_message>
add corrected PCB files
</commit_message>
<xml_diff>
--- a/HyperRail/HyperRail_BOM.xlsx
+++ b/HyperRail/HyperRail_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorian Brusind\Documents\GitHub\PersonalProjects\HyperRail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18EB069C-1FFC-4554-8678-F053B98C1ED1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC0A438-A1F9-4717-BC30-93C322F2609C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9AA5CA3B-103F-4503-BB38-84DF181EF15E}"/>
   </bookViews>
@@ -1492,6 +1492,15 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="13" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="44" fontId="12" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="12" xfId="4" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1522,15 +1531,6 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="13" xfId="5"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="44" fontId="12" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="12" xfId="4" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -3698,7 +3698,7 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3721,16 +3721,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="47" t="s">
         <v>319</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
     </row>
     <row r="2" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
@@ -3760,12 +3760,12 @@
       <c r="I2" s="24" t="s">
         <v>320</v>
       </c>
-      <c r="K2" s="51" t="s">
+      <c r="K2" s="41" t="s">
         <v>205</v>
       </c>
-      <c r="L2" s="52">
+      <c r="L2" s="42">
         <f>SUM(Table13[Extended Price])</f>
-        <v>677.98813750308909</v>
+        <v>641.65493076923076</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -3777,11 +3777,11 @@
       </c>
       <c r="E3" s="7">
         <f>Mechanical!I30</f>
-        <v>115.58109270587524</v>
+        <v>126.62215625075713</v>
       </c>
       <c r="F3" s="7">
         <f>Table13[[#This Row],[Unit Price]]*Table13[[#This Row],[Quantity]]</f>
-        <v>231.16218541175047</v>
+        <v>253.24431250151426</v>
       </c>
       <c r="I3" t="s">
         <v>322</v>
@@ -3796,19 +3796,19 @@
       </c>
       <c r="E4" s="7">
         <f>Mechanical!I47</f>
-        <v>48.928748959055127</v>
+        <v>50.351527874015751</v>
       </c>
       <c r="F4" s="7">
         <f>Table13[[#This Row],[Unit Price]]*Table13[[#This Row],[Quantity]]</f>
-        <v>48.928748959055127</v>
+        <v>50.351527874015751</v>
       </c>
       <c r="I4" t="s">
         <v>322</v>
       </c>
-      <c r="K4" s="56" t="s">
+      <c r="K4" s="46" t="s">
         <v>352</v>
       </c>
-      <c r="L4" s="56"/>
+      <c r="L4" s="46"/>
     </row>
     <row r="5" spans="1:18" ht="27" thickTop="1" x14ac:dyDescent="0.4">
       <c r="C5" t="s">
@@ -3828,15 +3828,15 @@
       <c r="I5" t="s">
         <v>323</v>
       </c>
-      <c r="K5" s="39" t="s">
+      <c r="K5" s="48" t="s">
         <v>341</v>
       </c>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39" t="s">
+      <c r="L5" s="48"/>
+      <c r="M5" s="48" t="s">
         <v>342</v>
       </c>
-      <c r="N5" s="39"/>
-      <c r="P5" s="55" t="s">
+      <c r="N5" s="48"/>
+      <c r="P5" s="45" t="s">
         <v>350</v>
       </c>
       <c r="R5" t="s">
@@ -3861,29 +3861,29 @@
       <c r="I6" t="s">
         <v>323</v>
       </c>
-      <c r="K6" s="48" t="s">
+      <c r="K6" s="38" t="s">
         <v>334</v>
       </c>
-      <c r="L6" s="49">
-        <v>1.2749999999999999</v>
-      </c>
-      <c r="M6" s="48" t="s">
+      <c r="L6" s="39">
+        <v>1.5</v>
+      </c>
+      <c r="M6" s="38" t="s">
         <v>334</v>
       </c>
-      <c r="N6" s="49">
+      <c r="N6" s="39">
         <f>L6</f>
-        <v>1.2749999999999999</v>
-      </c>
-      <c r="P6" s="48" t="s">
+        <v>1.5</v>
+      </c>
+      <c r="P6" s="38" t="s">
         <v>334</v>
       </c>
       <c r="Q6">
         <f>N6*(N9+1)</f>
-        <v>2.5499999999999998</v>
+        <v>1.5</v>
       </c>
       <c r="R6">
         <f>Q6*3.28084</f>
-        <v>8.366142</v>
+        <v>4.9212600000000002</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -3904,29 +3904,29 @@
       <c r="I7" t="s">
         <v>323</v>
       </c>
-      <c r="K7" s="48" t="s">
+      <c r="K7" s="38" t="s">
         <v>335</v>
       </c>
-      <c r="L7" s="49">
-        <v>1.895</v>
-      </c>
-      <c r="M7" s="48" t="s">
+      <c r="L7" s="39">
+        <v>2</v>
+      </c>
+      <c r="M7" s="38" t="s">
         <v>335</v>
       </c>
-      <c r="N7" s="49">
+      <c r="N7" s="39">
         <f t="shared" ref="N7:N8" si="0">L7</f>
-        <v>1.895</v>
-      </c>
-      <c r="P7" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="38" t="s">
         <v>335</v>
       </c>
       <c r="Q7">
         <f>N7*(N9+1)</f>
-        <v>3.79</v>
+        <v>2</v>
       </c>
       <c r="R7">
         <f>Q7*3.28084</f>
-        <v>12.4343836</v>
+        <v>6.56168</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -3938,38 +3938,38 @@
       </c>
       <c r="E8" s="7">
         <f>Mechanical!I58</f>
-        <v>29.8962557480315</v>
+        <v>31.219090393700789</v>
       </c>
       <c r="F8" s="7">
         <f>Table13[[#This Row],[Unit Price]]*Table13[[#This Row],[Quantity]]</f>
-        <v>29.8962557480315</v>
+        <v>31.219090393700789</v>
       </c>
       <c r="I8" t="s">
         <v>322</v>
       </c>
-      <c r="K8" s="48" t="s">
+      <c r="K8" s="38" t="s">
         <v>336</v>
       </c>
-      <c r="L8" s="49">
-        <v>1.2749999999999999</v>
-      </c>
-      <c r="M8" s="48" t="s">
+      <c r="L8" s="39">
+        <v>2</v>
+      </c>
+      <c r="M8" s="38" t="s">
         <v>336</v>
       </c>
-      <c r="N8" s="49">
+      <c r="N8" s="39">
         <f t="shared" si="0"/>
-        <v>1.2749999999999999</v>
-      </c>
-      <c r="P8" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" s="38" t="s">
         <v>336</v>
       </c>
       <c r="Q8">
         <f>N8*(N9+1)</f>
-        <v>2.5499999999999998</v>
+        <v>2</v>
       </c>
       <c r="R8">
         <f>Q8*3.28084</f>
-        <v>8.366142</v>
+        <v>6.56168</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -3978,24 +3978,24 @@
       </c>
       <c r="D9">
         <f>N9</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="7">
         <f>Mechanical!I69</f>
-        <v>61.160947384251969</v>
+        <v>70.079789291338585</v>
       </c>
       <c r="F9" s="7">
         <f>Table13[[#This Row],[Unit Price]]*Table13[[#This Row],[Quantity]]</f>
-        <v>61.160947384251969</v>
+        <v>0</v>
       </c>
       <c r="I9" t="s">
         <v>322</v>
       </c>
-      <c r="M9" s="50" t="s">
+      <c r="M9" s="40" t="s">
         <v>343</v>
       </c>
       <c r="N9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4040,8 +4040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0E5AEB-69FF-447D-8154-D544AC848EA4}">
   <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4068,23 +4068,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="58.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -4989,39 +4989,39 @@
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="49" t="s">
         <v>205</v>
       </c>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
       <c r="I24" s="5">
         <f>SUM(Table1[Extended Price])</f>
         <v>27.140000000000004</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="51" t="s">
         <v>203</v>
       </c>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42"/>
-      <c r="N25" s="42"/>
-      <c r="O25" s="42"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="51"/>
+      <c r="L25" s="51"/>
+      <c r="M25" s="51"/>
+      <c r="N25" s="51"/>
+      <c r="O25" s="51"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -6156,39 +6156,39 @@
       <c r="O51" s="9"/>
     </row>
     <row r="52" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="40" t="s">
+      <c r="A52" s="49" t="s">
         <v>205</v>
       </c>
-      <c r="B52" s="40"/>
-      <c r="C52" s="40"/>
-      <c r="D52" s="40"/>
-      <c r="E52" s="40"/>
-      <c r="F52" s="40"/>
-      <c r="G52" s="40"/>
-      <c r="H52" s="40"/>
+      <c r="B52" s="49"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="49"/>
+      <c r="H52" s="49"/>
       <c r="I52" s="7">
         <f>SUM(Table2[Extended Price])</f>
         <v>34.43</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A53" s="43" t="s">
+      <c r="A53" s="52" t="s">
         <v>204</v>
       </c>
-      <c r="B53" s="43"/>
-      <c r="C53" s="43"/>
-      <c r="D53" s="43"/>
-      <c r="E53" s="43"/>
-      <c r="F53" s="43"/>
-      <c r="G53" s="43"/>
-      <c r="H53" s="43"/>
-      <c r="I53" s="43"/>
-      <c r="J53" s="43"/>
-      <c r="K53" s="43"/>
-      <c r="L53" s="43"/>
-      <c r="M53" s="43"/>
-      <c r="N53" s="43"/>
-      <c r="O53" s="43"/>
+      <c r="B53" s="52"/>
+      <c r="C53" s="52"/>
+      <c r="D53" s="52"/>
+      <c r="E53" s="52"/>
+      <c r="F53" s="52"/>
+      <c r="G53" s="52"/>
+      <c r="H53" s="52"/>
+      <c r="I53" s="52"/>
+      <c r="J53" s="52"/>
+      <c r="K53" s="52"/>
+      <c r="L53" s="52"/>
+      <c r="M53" s="52"/>
+      <c r="N53" s="52"/>
+      <c r="O53" s="52"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
@@ -6521,16 +6521,16 @@
       <c r="O62" s="12"/>
     </row>
     <row r="63" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="40" t="s">
+      <c r="A63" s="49" t="s">
         <v>205</v>
       </c>
-      <c r="B63" s="40"/>
-      <c r="C63" s="40"/>
-      <c r="D63" s="40"/>
-      <c r="E63" s="40"/>
-      <c r="F63" s="40"/>
-      <c r="G63" s="40"/>
-      <c r="H63" s="40"/>
+      <c r="B63" s="49"/>
+      <c r="C63" s="49"/>
+      <c r="D63" s="49"/>
+      <c r="E63" s="49"/>
+      <c r="F63" s="49"/>
+      <c r="G63" s="49"/>
+      <c r="H63" s="49"/>
       <c r="I63" s="7">
         <f>SUM(Table5[Extended Price])</f>
         <v>163.85000000000002</v>
@@ -6634,8 +6634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A8BB3BB-C29D-41B2-82D5-D9E5E331DAA0}">
   <dimension ref="A1:AF69"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="I17" sqref="A17:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6659,23 +6659,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="55.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="54" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
       <c r="Q1" s="19" t="s">
         <v>0</v>
       </c>
@@ -7032,39 +7032,39 @@
       </c>
     </row>
     <row r="8" spans="1:32" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="49" t="s">
         <v>205</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
       <c r="I8" s="5">
         <f>SUM(RBA[Extended Price])</f>
         <v>3.9367946456692913</v>
       </c>
     </row>
     <row r="10" spans="1:32" ht="60.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="55" t="s">
         <v>231</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="46"/>
-      <c r="N10" s="46"/>
-      <c r="O10" s="46"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="55"/>
+      <c r="O10" s="55"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
@@ -7231,7 +7231,7 @@
       </c>
       <c r="G14">
         <f>Overall!L8*1000</f>
-        <v>1275</v>
+        <v>2000</v>
       </c>
       <c r="H14" s="5">
         <f>0.28/25.4</f>
@@ -7239,7 +7239,7 @@
       </c>
       <c r="I14" s="5">
         <f>SRA[[#This Row],[Quantity]]*SRA[[#This Row],[Unit Price]]</f>
-        <v>14.055118110236222</v>
+        <v>22.047244094488192</v>
       </c>
       <c r="J14" t="s">
         <v>235</v>
@@ -7284,7 +7284,7 @@
       </c>
       <c r="G15">
         <f>Overall!L6*1000</f>
-        <v>1275</v>
+        <v>1500</v>
       </c>
       <c r="H15" s="5">
         <f>0.28/25.4</f>
@@ -7292,7 +7292,7 @@
       </c>
       <c r="I15" s="5">
         <f>SRA[[#This Row],[Quantity]]*SRA[[#This Row],[Unit Price]]</f>
-        <v>14.055118110236222</v>
+        <v>16.535433070866144</v>
       </c>
       <c r="J15" t="s">
         <v>235</v>
@@ -7733,7 +7733,7 @@
       </c>
       <c r="G24">
         <f>ROUND(Overall!L6*1000*1.15,1)</f>
-        <v>1466.3</v>
+        <v>1725</v>
       </c>
       <c r="H24" s="5">
         <f>10.99/5000</f>
@@ -7741,7 +7741,7 @@
       </c>
       <c r="I24" s="30">
         <f>SRA[[#This Row],[Quantity]]*SRA[[#This Row],[Unit Price]]</f>
-        <v>3.2229273999999997</v>
+        <v>3.79155</v>
       </c>
       <c r="J24" t="s">
         <v>235</v>
@@ -7930,39 +7930,39 @@
       <c r="I29" s="30"/>
     </row>
     <row r="30" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="49" t="s">
         <v>205</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
       <c r="I30" s="5">
         <f>SUM(SRA[Extended Price])</f>
-        <v>115.58109270587524</v>
+        <v>126.62215625075713</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="47" t="s">
+      <c r="A32" s="56" t="s">
         <v>290</v>
       </c>
-      <c r="B32" s="47"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="47"/>
-      <c r="L32" s="47"/>
-      <c r="M32" s="47"/>
-      <c r="N32" s="47"/>
-      <c r="O32" s="47"/>
+      <c r="B32" s="56"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="56"/>
+      <c r="K32" s="56"/>
+      <c r="L32" s="56"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+      <c r="O32" s="56"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
@@ -8587,7 +8587,7 @@
       </c>
       <c r="G45" s="31">
         <f>ROUND(Overall!L7*1000*1.15,1)</f>
-        <v>2179.3000000000002</v>
+        <v>2300</v>
       </c>
       <c r="H45" s="34">
         <f>10.99/5000</f>
@@ -8595,7 +8595,7 @@
       </c>
       <c r="I45" s="33">
         <f>TCA[[#This Row],[Quantity]]*TCA[[#This Row],[Unit Price]]</f>
-        <v>4.7901014000000002</v>
+        <v>5.0553999999999997</v>
       </c>
       <c r="J45" t="s">
         <v>235</v>
@@ -8640,7 +8640,7 @@
       </c>
       <c r="G46" s="31">
         <f>Overall!L7*1000</f>
-        <v>1895</v>
+        <v>2000</v>
       </c>
       <c r="H46" s="34">
         <f>0.28/25.4</f>
@@ -8648,7 +8648,7 @@
       </c>
       <c r="I46" s="33">
         <f>TCA[[#This Row],[Quantity]]*TCA[[#This Row],[Unit Price]]</f>
-        <v>20.889763779527563</v>
+        <v>22.047244094488192</v>
       </c>
       <c r="J46" t="s">
         <v>235</v>
@@ -8673,39 +8673,39 @@
       </c>
     </row>
     <row r="47" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="40" t="s">
+      <c r="A47" s="49" t="s">
         <v>205</v>
       </c>
-      <c r="B47" s="40"/>
-      <c r="C47" s="40"/>
-      <c r="D47" s="40"/>
-      <c r="E47" s="40"/>
-      <c r="F47" s="40"/>
-      <c r="G47" s="40"/>
-      <c r="H47" s="40"/>
+      <c r="B47" s="49"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="49"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="49"/>
+      <c r="H47" s="49"/>
       <c r="I47" s="5">
         <f>SUM(TCA[Extended Price])</f>
-        <v>48.928748959055127</v>
+        <v>50.351527874015751</v>
       </c>
     </row>
     <row r="49" spans="1:16" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="44" t="s">
+      <c r="A49" s="53" t="s">
         <v>325</v>
       </c>
-      <c r="B49" s="44"/>
-      <c r="C49" s="44"/>
-      <c r="D49" s="44"/>
-      <c r="E49" s="44"/>
-      <c r="F49" s="44"/>
-      <c r="G49" s="44"/>
-      <c r="H49" s="44"/>
-      <c r="I49" s="44"/>
-      <c r="J49" s="44"/>
-      <c r="K49" s="44"/>
-      <c r="L49" s="44"/>
-      <c r="M49" s="44"/>
-      <c r="N49" s="44"/>
-      <c r="O49" s="44"/>
+      <c r="B49" s="53"/>
+      <c r="C49" s="53"/>
+      <c r="D49" s="53"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="53"/>
+      <c r="G49" s="53"/>
+      <c r="H49" s="53"/>
+      <c r="I49" s="53"/>
+      <c r="J49" s="53"/>
+      <c r="K49" s="53"/>
+      <c r="L49" s="53"/>
+      <c r="M49" s="53"/>
+      <c r="N49" s="53"/>
+      <c r="O49" s="53"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="23" t="s">
@@ -8882,7 +8882,7 @@
       </c>
       <c r="G53" s="31">
         <f>Overall!L7*1000*2</f>
-        <v>3790</v>
+        <v>4000</v>
       </c>
       <c r="H53" s="34">
         <f t="shared" ref="H53" si="1">0.16/25.4</f>
@@ -8890,7 +8890,7 @@
       </c>
       <c r="I53" s="5">
         <f>MMM[[#This Row],[Unit Price]]*MMM[[#This Row],[Quantity]]</f>
-        <v>23.8740157480315</v>
+        <v>25.196850393700789</v>
       </c>
       <c r="J53" t="s">
         <v>235</v>
@@ -9121,39 +9121,39 @@
       </c>
     </row>
     <row r="58" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="40" t="s">
+      <c r="A58" s="49" t="s">
         <v>205</v>
       </c>
-      <c r="B58" s="40"/>
-      <c r="C58" s="40"/>
-      <c r="D58" s="40"/>
-      <c r="E58" s="40"/>
-      <c r="F58" s="40"/>
-      <c r="G58" s="40"/>
-      <c r="H58" s="40"/>
+      <c r="B58" s="49"/>
+      <c r="C58" s="49"/>
+      <c r="D58" s="49"/>
+      <c r="E58" s="49"/>
+      <c r="F58" s="49"/>
+      <c r="G58" s="49"/>
+      <c r="H58" s="49"/>
       <c r="I58" s="5">
         <f>SUM(MMM[Extended Price])</f>
-        <v>29.8962557480315</v>
+        <v>31.219090393700789</v>
       </c>
     </row>
     <row r="60" spans="1:16" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="45" t="s">
+      <c r="A60" s="54" t="s">
         <v>337</v>
       </c>
-      <c r="B60" s="45"/>
-      <c r="C60" s="45"/>
-      <c r="D60" s="45"/>
-      <c r="E60" s="45"/>
-      <c r="F60" s="45"/>
-      <c r="G60" s="45"/>
-      <c r="H60" s="45"/>
-      <c r="I60" s="45"/>
-      <c r="J60" s="45"/>
-      <c r="K60" s="45"/>
-      <c r="L60" s="45"/>
-      <c r="M60" s="45"/>
-      <c r="N60" s="45"/>
-      <c r="O60" s="45"/>
+      <c r="B60" s="54"/>
+      <c r="C60" s="54"/>
+      <c r="D60" s="54"/>
+      <c r="E60" s="54"/>
+      <c r="F60" s="54"/>
+      <c r="G60" s="54"/>
+      <c r="H60" s="54"/>
+      <c r="I60" s="54"/>
+      <c r="J60" s="54"/>
+      <c r="K60" s="54"/>
+      <c r="L60" s="54"/>
+      <c r="M60" s="54"/>
+      <c r="N60" s="54"/>
+      <c r="O60" s="54"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="23" t="s">
@@ -9227,7 +9227,7 @@
       <c r="G62" s="27">
         <v>64</v>
       </c>
-      <c r="H62" s="53">
+      <c r="H62" s="43">
         <f>(16.68/100)</f>
         <v>0.1668</v>
       </c>
@@ -9277,7 +9277,7 @@
       <c r="G63" s="27">
         <v>64</v>
       </c>
-      <c r="H63" s="53">
+      <c r="H63" s="43">
         <f>9.49/100</f>
         <v>9.4899999999999998E-2</v>
       </c>
@@ -9328,7 +9328,7 @@
       </c>
       <c r="G64">
         <f>Overall!L8*1000</f>
-        <v>1275</v>
+        <v>2000</v>
       </c>
       <c r="H64" s="5">
         <f>0.28/25.4</f>
@@ -9336,7 +9336,7 @@
       </c>
       <c r="I64" s="5">
         <f>AOM[[#This Row],[Unit Price]]*AOM[[#This Row],[Quantity]]</f>
-        <v>14.055118110236222</v>
+        <v>22.047244094488192</v>
       </c>
       <c r="J64" t="s">
         <v>235</v>
@@ -9381,15 +9381,15 @@
       </c>
       <c r="G65" s="37">
         <f>Overall!L7*1000</f>
-        <v>1895</v>
-      </c>
-      <c r="H65" s="54">
+        <v>2000</v>
+      </c>
+      <c r="H65" s="44">
         <f t="shared" ref="H65" si="2">0.16/25.4</f>
         <v>6.2992125984251976E-3</v>
       </c>
       <c r="I65" s="5">
         <f>AOM[[#This Row],[Unit Price]]*AOM[[#This Row],[Quantity]]</f>
-        <v>11.93700787401575</v>
+        <v>12.598425196850394</v>
       </c>
       <c r="J65" t="s">
         <v>235</v>
@@ -9434,7 +9434,7 @@
       </c>
       <c r="G66" s="37">
         <f>ROUND(Overall!L7*1000*1.15,1)</f>
-        <v>2179.3000000000002</v>
+        <v>2300</v>
       </c>
       <c r="H66" s="32">
         <f>10.99/5000</f>
@@ -9442,7 +9442,7 @@
       </c>
       <c r="I66" s="5">
         <f>AOM[[#This Row],[Unit Price]]*AOM[[#This Row],[Quantity]]</f>
-        <v>4.7901014000000002</v>
+        <v>5.0553999999999997</v>
       </c>
       <c r="J66" t="s">
         <v>235</v>
@@ -9488,7 +9488,7 @@
       <c r="G67" s="27">
         <v>2</v>
       </c>
-      <c r="H67" s="53">
+      <c r="H67" s="43">
         <f>22.64*0.089</f>
         <v>2.0149599999999999</v>
       </c>
@@ -9540,7 +9540,7 @@
       <c r="G68" s="27">
         <v>8</v>
       </c>
-      <c r="H68" s="53">
+      <c r="H68" s="43">
         <v>1.2</v>
       </c>
       <c r="I68" s="5">
@@ -9567,19 +9567,19 @@
       </c>
     </row>
     <row r="69" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="40" t="s">
+      <c r="A69" s="49" t="s">
         <v>205</v>
       </c>
-      <c r="B69" s="40"/>
-      <c r="C69" s="40"/>
-      <c r="D69" s="40"/>
-      <c r="E69" s="40"/>
-      <c r="F69" s="40"/>
-      <c r="G69" s="40"/>
-      <c r="H69" s="40"/>
+      <c r="B69" s="49"/>
+      <c r="C69" s="49"/>
+      <c r="D69" s="49"/>
+      <c r="E69" s="49"/>
+      <c r="F69" s="49"/>
+      <c r="G69" s="49"/>
+      <c r="H69" s="49"/>
       <c r="I69" s="5">
         <f>SUM(AOM[Extended Price])</f>
-        <v>61.160947384251969</v>
+        <v>70.079789291338585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>